<commit_message>
Passive x Active modes
Two different types of cards were add
</commit_message>
<xml_diff>
--- a/Espanol.xlsx
+++ b/Espanol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Outros computadores\São Carlos\Backup\São Carlos\USP\Programação\CardMaker-Pro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Outros computadores\São Carlos\Backup\São Carlos\USP\Programação\GitHub\CardMaker-Pro\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9648FEB-6AA5-4114-8FC0-8218D621BB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7324A3-2EF6-477E-84C9-EB09D60C9A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17256" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,64 +25,253 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
-  <si>
-    <t>¿Cuáles son los hechos de su historia?</t>
-  </si>
-  <si>
-    <t>Es tu hermano, debes ayudarlo</t>
-  </si>
-  <si>
-    <t>Se tardó un año en completar la traducción de la novela.</t>
-  </si>
-  <si>
-    <t>Para ganar un partido de tenis, un jugador debe tener una ventaja de dos puntos.</t>
-  </si>
-  <si>
-    <t>La sopa está ligeramente salada.</t>
-  </si>
-  <si>
-    <t>¿Me puede explicar cómo funciona?</t>
-  </si>
-  <si>
-    <t>Ella diseña software para organizar los asientos en restaurantes.</t>
-  </si>
-  <si>
-    <t>¿Has descargado el podcast más reciente?</t>
-  </si>
-  <si>
-    <t>Tenemos un camino largo por delante para llegar a casa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siempre es mejor consultar a un traductor que una traducción automática. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haz una copia de seguridad de tus archivos </t>
-  </si>
-  <si>
-    <t>Tengo las contraseñas de todas mis cuentas de correo electrónico memorizadas.</t>
-  </si>
-  <si>
-    <t>En cualquier caso, su decisión es firme</t>
-  </si>
-  <si>
-    <t>Es un milagro que se haya curado.</t>
-  </si>
-  <si>
-    <t>Front</t>
-  </si>
-  <si>
-    <t>Back</t>
-  </si>
-  <si>
-    <t>active</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Señor Presidente, voy a hacer algo inusual, pero creo que es necesario.</t>
+  </si>
+  <si>
+    <t>No sé qué había ocurrido, pero Mauricio parecía agitado; hablaba muy rápido</t>
+  </si>
+  <si>
+    <t>Danos tiempo para reflexionar sobre ello.</t>
+  </si>
+  <si>
+    <t>Hablé sin pensar.</t>
+  </si>
+  <si>
+    <t>No quiero ni imaginarme lo que podría haber pasado.</t>
+  </si>
+  <si>
+    <r>
+      <t>Puede leer un </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>informe científico</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> del descubrimiento en el sitio web de la UNESCO.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>En el mar, tu vida podría </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>depender</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> de estas cosas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ya no hace </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>falta hacer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> más preguntas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Aún me </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>falta hacer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> la mitad</t>
+    </r>
+  </si>
+  <si>
+    <t>¿Tu amigo todavía vive en Londres?</t>
+  </si>
+  <si>
+    <t>Aún no habían empezado a comer cuando llegué.</t>
+  </si>
+  <si>
+    <r>
+      <t>La siguiente clasificación de emociones fue </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>hecha por</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> Parrott, W.</t>
+    </r>
+  </si>
+  <si>
+    <t>No hay suficiente memoria RAM en tu ordenador para ejecutar este programa.</t>
+  </si>
+  <si>
+    <t>La incertidumbre de la duración de nuestra vida, puede motivar a alguno de nosotros a realizar un gran esfuerzo.</t>
+  </si>
+  <si>
+    <r>
+      <t>El </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>signo más menos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> es un símbolo matemático que se emplea a menudo para indicar la </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0645AD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>precisión</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202122"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> de una </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0645AD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>aproximación</t>
+    </r>
+  </si>
+  <si>
+    <t>Una desviación estándar baja indica que la mayor parte de los datos de una muestra tienden a estar agrupados cerca de su media</t>
+  </si>
+  <si>
+    <t>Copia el archivo en la carpeta deseada.</t>
+  </si>
+  <si>
+    <t>El río crece mucho durante la época de lluvias.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> la entropía es una magnitud física para un sistema termodinámico en equilibrio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permitiendo formular expresiones de la forma si y solo si </t>
+  </si>
+  <si>
+    <t>Si el dividendo es 12 y el divisor es 6, entonces el cociente es 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Um julio es aproximadamente la energía necesaria para lanzar una manzana </t>
+  </si>
+  <si>
+    <t>No obstante, sumando un término positivo al segundo miembro, podemos transformar de nuevo la expresión en una ecuación</t>
+  </si>
+  <si>
+    <t>Se denomina calor a la energía en tránsito en um sistema termodinamico</t>
+  </si>
+  <si>
+    <t>Los sistemas termodinámicos se clasifican según el grado de aislamiento que presentan con su entorno.</t>
+  </si>
+  <si>
+    <t>Los alumnos tienen que cumplir las normas del colegio</t>
+  </si>
+  <si>
+    <t>En la expansión isotérmica de un gas, todo el calor absorbido del medio se transforma en trabajo</t>
+  </si>
+  <si>
+    <t>Si se trata de un proceso reversible, la variacion de entropia es cero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,16 +285,72 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0970AC"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0645AD"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,15 +358,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE9E9E9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,140 +669,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="34.77734375" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="105.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>13</v>
+    </row>
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A17" r:id="rId1" tooltip="Media (matemáticas)" display="https://es.wikipedia.org/wiki/Media_(matem%C3%A1ticas)" xr:uid="{0DE21A97-B230-47F0-B9E1-C2232150F19B}"/>
+    <hyperlink ref="A25" r:id="rId2" tooltip="Sistema termodinámico" display="https://es.wikipedia.org/wiki/Sistema_termodin%C3%A1mico" xr:uid="{7CD1FF20-F958-4A42-A1AB-0A69A6825209}"/>
+    <hyperlink ref="A29" r:id="rId3" tooltip="Proceso reversible" display="https://es.wikipedia.org/wiki/Proceso_reversible" xr:uid="{D61FF7A5-8FEE-4CDE-9ED0-6BEAD4DC17FC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>